<commit_message>
nesten ferdig med statetikktabell
</commit_message>
<xml_diff>
--- a/data/Regning av kaloriforbruk.xlsx
+++ b/data/Regning av kaloriforbruk.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c3fb2a472a4d152/Skrivebord/R/Master/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c3fb2a472a4d152/Skrivebord/R/Master/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="11_F25DC773A252ABDACC1048E1A95861305ADE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34E78053-3173-4A89-AB2A-C6B2B3FB39BE}"/>
+  <xr:revisionPtr revIDLastSave="226" documentId="11_F25DC773A252ABDACC1048E1A95861305ADE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C9156D-3421-4924-BCB9-C7167F257AF9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="240" windowWidth="19200" windowHeight="9840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -240,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -255,6 +255,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -270,6 +271,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,7 +557,7 @@
     <col min="12" max="12" width="23.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +586,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -608,12 +613,12 @@
         <f>E2*4.939</f>
         <v>6.2067425200000006</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="4">
         <f>H2*4.182</f>
         <v>25.956597218640006</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -640,12 +645,18 @@
         <f>E3*5.003</f>
         <v>6.7526491600000007</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="4">
         <f t="shared" ref="I3:I66" si="1">H3*4.182</f>
         <v>28.239578787120006</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K3" s="8">
+        <v>1256.68</v>
+      </c>
+      <c r="L3" s="8">
+        <v>1324.56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -672,12 +683,18 @@
         <f>E4*4.927</f>
         <v>5.8723927599999994</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="4">
         <f t="shared" si="1"/>
         <v>24.558346522320001</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K4" s="8">
+        <v>1349.72</v>
+      </c>
+      <c r="L4" s="8">
+        <v>1198.72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -704,12 +721,18 @@
         <f>E5*4.927</f>
         <v>7.04521584</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="4">
         <f t="shared" si="1"/>
         <v>29.463092642880003</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K5" s="8">
+        <v>1191.8800000000001</v>
+      </c>
+      <c r="L5" s="8">
+        <v>1095.52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -736,12 +759,18 @@
         <f>E6*4.939</f>
         <v>6.5847606956521734</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="4">
         <f t="shared" si="1"/>
         <v>27.537469229217393</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K6" s="8">
+        <v>1044.08</v>
+      </c>
+      <c r="L6" s="8">
+        <v>1117.44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -768,12 +797,18 @@
         <f>E7*5.014</f>
         <v>6.1339270400000006</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="4">
         <f t="shared" si="1"/>
         <v>25.652082881280005</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K7" s="8">
+        <v>1508.4</v>
+      </c>
+      <c r="L7" s="8">
+        <v>1503.76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -800,12 +835,18 @@
         <f>E8*4.968</f>
         <v>11.914655040000001</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="4">
         <f t="shared" si="1"/>
         <v>49.827087377280009</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K8" s="8">
+        <v>1738.3157894736842</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1377.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -832,12 +873,18 @@
         <f>E9*5.003</f>
         <v>5.2235322399999999</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="4">
         <f t="shared" si="1"/>
         <v>21.844811827680001</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K9" s="8">
+        <v>1397.2</v>
+      </c>
+      <c r="L9" s="8">
+        <v>1592.72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -864,12 +911,18 @@
         <f>E10*4.863</f>
         <v>7.2538453200000008</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="4">
         <f t="shared" si="1"/>
         <v>30.335581128240005</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K10" s="8">
+        <v>1155.1600000000001</v>
+      </c>
+      <c r="L10" s="8">
+        <v>1305.96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -896,12 +949,18 @@
         <f>E11*4.904</f>
         <v>4.6168217600000006</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="4">
         <f t="shared" si="1"/>
         <v>19.307548600320004</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K11" s="8">
+        <v>1149.92</v>
+      </c>
+      <c r="L11" s="8">
+        <v>1314.84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -928,12 +987,18 @@
         <f>E12*4.951</f>
         <v>6.0439827599999996</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="4">
         <f t="shared" si="1"/>
         <v>25.275935902320001</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K12" s="8">
+        <v>1242.6400000000001</v>
+      </c>
+      <c r="L12" s="8">
+        <v>1175.92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -960,12 +1025,18 @@
         <f>E13*4.939</f>
         <v>5.7956201600000004</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="4">
         <f t="shared" si="1"/>
         <v>24.237283509120005</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K13" s="8">
+        <v>1135.28</v>
+      </c>
+      <c r="L13" s="8">
+        <v>1145.56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -992,12 +1063,12 @@
         <f>E14*5.055</f>
         <v>7.6249620000000009</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="4">
         <f t="shared" si="1"/>
         <v>31.887591084000007</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1024,12 +1095,12 @@
         <f>E15*5.003</f>
         <v>6.6505879599999993</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="4">
         <f t="shared" si="1"/>
         <v>27.812758848719998</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1056,12 +1127,13 @@
         <f>E16*4.985</f>
         <v>7.8332296000000001</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="4">
         <f t="shared" si="1"/>
         <v>32.758566187200003</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1088,12 +1160,12 @@
         <f>E17*4.98</f>
         <v>6.2977080000000001</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="4">
         <f t="shared" si="1"/>
         <v>26.337014856000003</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1120,12 +1192,13 @@
         <f>E18*5.043</f>
         <v>5.6110435200000008</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="4">
         <f t="shared" si="1"/>
         <v>23.465384000640007</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1151,11 +1224,11 @@
       <c r="H19" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1182,12 +1255,12 @@
         <f>E20*4.881</f>
         <v>7.3027569600000009</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="4">
         <f t="shared" si="1"/>
         <v>30.540129606720008</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1214,12 +1287,12 @@
         <f>E21*4.958</f>
         <v>5.5357061600000002</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="4">
         <f t="shared" si="1"/>
         <v>23.150323161120003</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1246,12 +1319,12 @@
         <f>E22*4.927</f>
         <v>6.8840043999999994</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="4">
         <f t="shared" si="1"/>
         <v>28.788906400799998</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1278,12 +1351,12 @@
         <f>E23*4.945</f>
         <v>7.7440677999999998</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="4">
         <f t="shared" si="1"/>
         <v>32.385691539600003</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1310,12 +1383,12 @@
         <f>E24*5.003</f>
         <v>5.3960356799999998</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="4">
         <f t="shared" si="1"/>
         <v>22.566221213760002</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1342,12 +1415,12 @@
         <f>E25*4.956</f>
         <v>8.559012000000001</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="4">
         <f t="shared" si="1"/>
         <v>35.793788184000007</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1374,12 +1447,12 @@
         <f>E26*5.072</f>
         <v>6.9111071999999991</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="4">
         <f t="shared" si="1"/>
         <v>28.902250310399999</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1406,12 +1479,12 @@
         <f>E27*5.003</f>
         <v>5.4284551199999997</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="4">
         <f t="shared" si="1"/>
         <v>22.701799311840002</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1438,12 +1511,12 @@
         <f>E28*5.037</f>
         <v>5.8185409200000011</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="4">
         <f t="shared" si="1"/>
         <v>24.333138127440005</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1470,12 +1543,12 @@
         <f>E29*4.991</f>
         <v>6.9961841599999994</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="4">
         <f t="shared" si="1"/>
         <v>29.258042157120002</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1502,12 +1575,12 @@
         <f>E30*5.014</f>
         <v>9.0247821666666681</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="4">
         <f t="shared" si="1"/>
         <v>37.741639021000012</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1534,12 +1607,12 @@
         <f>E31*4.899</f>
         <v>5.6334580800000005</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="4">
         <f t="shared" si="1"/>
         <v>23.559121690560005</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1566,7 +1639,7 @@
         <f>E32*5.06</f>
         <v>6.2877584000000004</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="4">
         <f t="shared" si="1"/>
         <v>26.295405628800005</v>
       </c>
@@ -1598,7 +1671,7 @@
         <f>E33*5.003</f>
         <v>5.3798259599999989</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="4">
         <f t="shared" si="1"/>
         <v>22.498432164719997</v>
       </c>
@@ -1630,7 +1703,7 @@
         <f>E34*4.951</f>
         <v>6.1012163199999989</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="4">
         <f t="shared" si="1"/>
         <v>25.515286650239997</v>
       </c>
@@ -1662,7 +1735,7 @@
         <f>E35*4.974</f>
         <v>7.5670456800000006</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="4">
         <f t="shared" si="1"/>
         <v>31.645385033760004</v>
       </c>
@@ -1694,7 +1767,7 @@
         <f>E36*5.008</f>
         <v>5.6854822400000007</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="4">
         <f t="shared" si="1"/>
         <v>23.776686727680005</v>
       </c>
@@ -1726,7 +1799,7 @@
         <f>E37*5.037</f>
         <v>4.7486821199999998</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="4">
         <f t="shared" si="1"/>
         <v>19.858988625840002</v>
       </c>
@@ -1758,7 +1831,7 @@
         <f>E38*5.02</f>
         <v>5.5515176000000004</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="4">
         <f t="shared" si="1"/>
         <v>23.216446603200005</v>
       </c>
@@ -1790,7 +1863,7 @@
         <f>E39*4.991</f>
         <v>5.9075472399999995</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="4">
         <f t="shared" si="1"/>
         <v>24.705362557680001</v>
       </c>
@@ -1822,7 +1895,7 @@
         <f>E40*4.974</f>
         <v>6.5883614399999999</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="4">
         <f t="shared" si="1"/>
         <v>27.552527542080004</v>
       </c>
@@ -1854,7 +1927,7 @@
         <f>E41*4.927</f>
         <v>5.9242248000000002</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="4">
         <f t="shared" si="1"/>
         <v>24.775108113600002</v>
       </c>
@@ -1886,7 +1959,7 @@
         <f>E42*4.962</f>
         <v>5.9480486399999997</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="4">
         <f t="shared" si="1"/>
         <v>24.87473941248</v>
       </c>
@@ -1918,7 +1991,7 @@
         <f>E43*4.962</f>
         <v>5.4359702399999996</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="4">
         <f t="shared" si="1"/>
         <v>22.733227543680002</v>
       </c>
@@ -1950,7 +2023,7 @@
         <f>E44*5.014</f>
         <v>4.3206640800000002</v>
       </c>
-      <c r="I44">
+      <c r="I44" s="4">
         <f t="shared" si="1"/>
         <v>18.069017182560003</v>
       </c>
@@ -1982,7 +2055,7 @@
         <f>E45*5.037</f>
         <v>5.8112876400000006</v>
       </c>
-      <c r="I45">
+      <c r="I45" s="4">
         <f t="shared" si="1"/>
         <v>24.302804910480006</v>
       </c>
@@ -2014,7 +2087,7 @@
         <f>E46*4.991</f>
         <v>7.5423992000000002</v>
       </c>
-      <c r="I46">
+      <c r="I46" s="4">
         <f t="shared" si="1"/>
         <v>31.542313454400002</v>
       </c>
@@ -2046,7 +2119,7 @@
         <f>E47*5.055</f>
         <v>5.9183940000000002</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="4">
         <f t="shared" si="1"/>
         <v>24.750723708000002</v>
       </c>
@@ -2078,7 +2151,7 @@
         <f>E48*4.974</f>
         <v>5.55814656</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="4">
         <f t="shared" si="1"/>
         <v>23.244168913920003</v>
       </c>
@@ -2110,7 +2183,7 @@
         <f>E49*5.037</f>
         <v>6.5701368750000002</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="4">
         <f t="shared" si="1"/>
         <v>27.476312411250003</v>
       </c>
@@ -2142,7 +2215,7 @@
         <f>E50*4.945</f>
         <v>6.1606100000000001</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="4">
         <f t="shared" si="1"/>
         <v>25.763671020000004</v>
       </c>
@@ -2174,7 +2247,7 @@
         <f>E51*4.922</f>
         <v>5.3848730833333338</v>
       </c>
-      <c r="I51">
+      <c r="I51" s="4">
         <f t="shared" si="1"/>
         <v>22.519539234500005</v>
       </c>
@@ -2206,7 +2279,7 @@
         <f>E52*5.026</f>
         <v>7.5578977599999995</v>
       </c>
-      <c r="I52">
+      <c r="I52" s="4">
         <f t="shared" si="1"/>
         <v>31.60712843232</v>
       </c>
@@ -2238,7 +2311,7 @@
         <f>E53*4.985</f>
         <v>7.9355218000000018</v>
       </c>
-      <c r="I53">
+      <c r="I53" s="4">
         <f t="shared" si="1"/>
         <v>33.186352167600013</v>
       </c>
@@ -2270,7 +2343,7 @@
         <f>E54*4.974</f>
         <v>7.2737786399999997</v>
       </c>
-      <c r="I54">
+      <c r="I54" s="4">
         <f t="shared" si="1"/>
         <v>30.418942272480002</v>
       </c>
@@ -2302,7 +2375,7 @@
         <f>E55*4.933</f>
         <v>6.4077696800000004</v>
       </c>
-      <c r="I55">
+      <c r="I55" s="4">
         <f t="shared" si="1"/>
         <v>26.797292801760005</v>
       </c>
@@ -2334,7 +2407,7 @@
         <f>E56*5.02</f>
         <v>4.8220111999999995</v>
       </c>
-      <c r="I56">
+      <c r="I56" s="4">
         <f t="shared" si="1"/>
         <v>20.165650838400001</v>
       </c>
@@ -2366,7 +2439,7 @@
         <f>E57*4.893</f>
         <v>6.7386396</v>
       </c>
-      <c r="I57">
+      <c r="I57" s="4">
         <f t="shared" si="1"/>
         <v>28.180990807200004</v>
       </c>
@@ -2398,7 +2471,7 @@
         <f>E58*4.951</f>
         <v>7.8855567200000003</v>
       </c>
-      <c r="I58">
+      <c r="I58" s="4">
         <f t="shared" si="1"/>
         <v>32.977398203040003</v>
       </c>
@@ -2430,7 +2503,7 @@
         <f>E59*5.049</f>
         <v>7.8802772399999998</v>
       </c>
-      <c r="I59">
+      <c r="I59" s="4">
         <f t="shared" si="1"/>
         <v>32.955319417680002</v>
       </c>
@@ -2462,7 +2535,7 @@
         <f>E60*5.003</f>
         <v>8.3654329166666663</v>
       </c>
-      <c r="I60">
+      <c r="I60" s="4">
         <f t="shared" si="1"/>
         <v>34.9842404575</v>
       </c>
@@ -2494,7 +2567,7 @@
         <f>E61*4.933</f>
         <v>6.4423006799999998</v>
       </c>
-      <c r="I61">
+      <c r="I61" s="4">
         <f t="shared" si="1"/>
         <v>26.941701443760003</v>
       </c>
@@ -2526,7 +2599,7 @@
         <f>E62*5.072</f>
         <v>6.2174604799999988</v>
       </c>
-      <c r="I62">
+      <c r="I62" s="4">
         <f t="shared" si="1"/>
         <v>26.001419727359998</v>
       </c>
@@ -2558,7 +2631,7 @@
         <f>E63*4.968</f>
         <v>5.6750457599999997</v>
       </c>
-      <c r="I63">
+      <c r="I63" s="4">
         <f t="shared" si="1"/>
         <v>23.733041368320002</v>
       </c>
@@ -2588,7 +2661,7 @@
       <c r="H64" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="I64" s="7" t="s">
+      <c r="I64" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -2619,7 +2692,7 @@
         <f>E65*5.078</f>
         <v>6.6767575200000007</v>
       </c>
-      <c r="I65">
+      <c r="I65" s="4">
         <f t="shared" si="1"/>
         <v>27.922199948640007</v>
       </c>
@@ -2651,7 +2724,7 @@
         <f>E66*5.089</f>
         <v>5.8543856000000005</v>
       </c>
-      <c r="I66">
+      <c r="I66" s="4">
         <f t="shared" si="1"/>
         <v>24.483040579200004</v>
       </c>
@@ -2683,7 +2756,7 @@
         <f>E67*5.101</f>
         <v>5.9983679200000006</v>
       </c>
-      <c r="I67">
+      <c r="I67" s="4">
         <f t="shared" ref="I67:I70" si="3">H67*4.182</f>
         <v>25.085174641440005</v>
       </c>
@@ -2715,7 +2788,7 @@
         <f>E68*5.02</f>
         <v>6.5780071999999992</v>
       </c>
-      <c r="I68">
+      <c r="I68" s="4">
         <f t="shared" si="3"/>
         <v>27.5092261104</v>
       </c>
@@ -2747,7 +2820,7 @@
         <f>E69*4.945</f>
         <v>5.6647942000000002</v>
       </c>
-      <c r="I69">
+      <c r="I69" s="4">
         <f t="shared" si="3"/>
         <v>23.690169344400005</v>
       </c>
@@ -2779,7 +2852,7 @@
         <f>E70*4.916</f>
         <v>4.5830884800000007</v>
       </c>
-      <c r="I70">
+      <c r="I70" s="4">
         <f t="shared" si="3"/>
         <v>19.166476023360005</v>
       </c>

</xml_diff>

<commit_message>
endringer i "endring" pluss ending i tall i resutltatskjema for å få gjort ITT
</commit_message>
<xml_diff>
--- a/data/Regning av kaloriforbruk.xlsx
+++ b/data/Regning av kaloriforbruk.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c3fb2a472a4d152/Skrivebord/R/Master/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="11_F25DC773A252ABDACC1048E1A95861305ADE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C9156D-3421-4924-BCB9-C7167F257AF9}"/>
+  <xr:revisionPtr revIDLastSave="227" documentId="11_F25DC773A252ABDACC1048E1A95861305ADE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F1ECAE7E-9CC9-4B70-97BD-697F1A65A400}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -271,10 +271,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -542,8 +538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3:L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -649,12 +645,8 @@
         <f t="shared" ref="I3:I66" si="1">H3*4.182</f>
         <v>28.239578787120006</v>
       </c>
-      <c r="K3" s="8">
-        <v>1256.68</v>
-      </c>
-      <c r="L3" s="8">
-        <v>1324.56</v>
-      </c>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -687,12 +679,8 @@
         <f t="shared" si="1"/>
         <v>24.558346522320001</v>
       </c>
-      <c r="K4" s="8">
-        <v>1349.72</v>
-      </c>
-      <c r="L4" s="8">
-        <v>1198.72</v>
-      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -725,12 +713,8 @@
         <f t="shared" si="1"/>
         <v>29.463092642880003</v>
       </c>
-      <c r="K5" s="8">
-        <v>1191.8800000000001</v>
-      </c>
-      <c r="L5" s="8">
-        <v>1095.52</v>
-      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -763,12 +747,8 @@
         <f t="shared" si="1"/>
         <v>27.537469229217393</v>
       </c>
-      <c r="K6" s="8">
-        <v>1044.08</v>
-      </c>
-      <c r="L6" s="8">
-        <v>1117.44</v>
-      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -801,12 +781,8 @@
         <f t="shared" si="1"/>
         <v>25.652082881280005</v>
       </c>
-      <c r="K7" s="8">
-        <v>1508.4</v>
-      </c>
-      <c r="L7" s="8">
-        <v>1503.76</v>
-      </c>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -839,12 +815,8 @@
         <f t="shared" si="1"/>
         <v>49.827087377280009</v>
       </c>
-      <c r="K8" s="8">
-        <v>1738.3157894736842</v>
-      </c>
-      <c r="L8" s="8">
-        <v>1377.2</v>
-      </c>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -877,12 +849,8 @@
         <f t="shared" si="1"/>
         <v>21.844811827680001</v>
       </c>
-      <c r="K9" s="8">
-        <v>1397.2</v>
-      </c>
-      <c r="L9" s="8">
-        <v>1592.72</v>
-      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -915,12 +883,8 @@
         <f t="shared" si="1"/>
         <v>30.335581128240005</v>
       </c>
-      <c r="K10" s="8">
-        <v>1155.1600000000001</v>
-      </c>
-      <c r="L10" s="8">
-        <v>1305.96</v>
-      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -953,12 +917,8 @@
         <f t="shared" si="1"/>
         <v>19.307548600320004</v>
       </c>
-      <c r="K11" s="8">
-        <v>1149.92</v>
-      </c>
-      <c r="L11" s="8">
-        <v>1314.84</v>
-      </c>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -991,12 +951,8 @@
         <f t="shared" si="1"/>
         <v>25.275935902320001</v>
       </c>
-      <c r="K12" s="8">
-        <v>1242.6400000000001</v>
-      </c>
-      <c r="L12" s="8">
-        <v>1175.92</v>
-      </c>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1029,12 +985,8 @@
         <f t="shared" si="1"/>
         <v>24.237283509120005</v>
       </c>
-      <c r="K13" s="8">
-        <v>1135.28</v>
-      </c>
-      <c r="L13" s="8">
-        <v>1145.56</v>
-      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">

</xml_diff>